<commit_message>
correct the xlsx example to have all columns required for sample template. add note for csv dates that cannot be converted
</commit_message>
<xml_diff>
--- a/frontend/public/docs/mssc-ches-merge-example.xlsx
+++ b/frontend/public/docs/mssc-ches-merge-example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Projects/parc-jason/nr-messaging-service-showcase/frontend/public/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04DF5350-B1AC-2643-9687-063A10D301A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D551AC0-1BCF-404D-9827-EC37F1472ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="-17880" windowWidth="28040" windowHeight="16700" xr2:uid="{1985E953-2689-D24D-821D-7FA853425D3C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Start Date</t>
   </si>
@@ -81,6 +81,69 @@
   </si>
   <si>
     <t>long tom</t>
+  </si>
+  <si>
+    <t>Greeting</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>#!@&amp;*Quote (?!)</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>You speak an infinite deal of nothing.</t>
+  </si>
+  <si>
+    <t>William Shakespeare</t>
+  </si>
+  <si>
+    <t>Bonjour</t>
+  </si>
+  <si>
+    <t>Monde</t>
+  </si>
+  <si>
+    <t>These violent delights have violent ends and in their triumph die, like fire and powder which, as they kiss, consume.</t>
+  </si>
+  <si>
+    <t>Ciao</t>
+  </si>
+  <si>
+    <t>Mondo</t>
+  </si>
+  <si>
+    <t>Conscience doth make cowards of us all.</t>
+  </si>
+  <si>
+    <t>Hallo</t>
+  </si>
+  <si>
+    <t>Welt</t>
+  </si>
+  <si>
+    <t>When tyranny becomes law, rebellion becomes duty.</t>
+  </si>
+  <si>
+    <t>Thomas Jefferson</t>
+  </si>
+  <si>
+    <t>Hola</t>
+  </si>
+  <si>
+    <t>Mundo</t>
+  </si>
+  <si>
+    <t>A true patriot will defend his country from its government.</t>
   </si>
 </sst>
 </file>
@@ -434,124 +497,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D604B0F-AE2F-2849-9383-409249657505}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" customWidth="1"/>
+    <col min="11" max="11" width="19.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1">
         <v>43742</v>
       </c>
-      <c r="B2" s="2">
+      <c r="F2" s="2">
         <v>43744.572916666664</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2">
+      <c r="K2" s="2">
         <v>43742.614583333336</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1">
         <v>43742</v>
       </c>
-      <c r="B3" s="2">
+      <c r="F3" s="2">
         <v>43744.572916666664</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1">
         <v>43742</v>
       </c>
-      <c r="B4" s="2">
+      <c r="F4" s="2">
         <v>43744.572916666664</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1">
         <v>43742</v>
       </c>
-      <c r="B5" s="2">
+      <c r="F5" s="2">
         <v>43744.572916666664</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2">
+      <c r="K5" s="2">
         <v>43742.614583333336</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1">
         <v>43742</v>
       </c>
-      <c r="B6" s="2">
+      <c r="F6" s="2">
         <v>43744.572916666664</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
+      <c r="J6" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>